<commit_message>
Start Project 2, fix dataset
</commit_message>
<xml_diff>
--- a/Project1/AirplaneCrashes.xlsx
+++ b/Project1/AirplaneCrashes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/School/CSE-332/Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{92D8B100-1BCD-1E43-99DA-765EC28ED5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4282AC-6A2A-E44E-99AD-50C5CFB1F55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="18880"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AirplaneCrashes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="1100">
   <si>
     <t>Date</t>
   </si>
@@ -3321,12 +3321,24 @@
   </si>
   <si>
     <t>Fatalities Passengers</t>
+  </si>
+  <si>
+    <t>Jellicoe, Ontario, Canada</t>
+  </si>
+  <si>
+    <t>Huron Air</t>
+  </si>
+  <si>
+    <t>de Havilland DHC-3 Otter</t>
+  </si>
+  <si>
+    <t>Crashed into Blackwater Lake shortly after taking off from a remote landing strip.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4162,11 +4174,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N250"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B219" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C256" sqref="C256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14788,6 +14800,47 @@
         <v>342</v>
       </c>
     </row>
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>37971</v>
+      </c>
+      <c r="B251" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F251" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G251">
+        <v>3</v>
+      </c>
+      <c r="H251">
+        <v>2</v>
+      </c>
+      <c r="I251">
+        <v>1</v>
+      </c>
+      <c r="J251">
+        <v>2</v>
+      </c>
+      <c r="K251">
+        <v>1</v>
+      </c>
+      <c r="L251">
+        <v>1</v>
+      </c>
+      <c r="M251">
+        <v>0</v>
+      </c>
+      <c r="N251" t="s">
+        <v>1099</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>